<commit_message>
Adding missing data files
</commit_message>
<xml_diff>
--- a/data/output/processing_statistics.xlsx
+++ b/data/output/processing_statistics.xlsx
@@ -461,11 +461,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_AC.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AC.csv.gz</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>350298</v>
+        <v>352928</v>
       </c>
     </row>
     <row r="3">
@@ -479,11 +479,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_AL.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AL.csv.gz</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1067917</v>
+        <v>1072791</v>
       </c>
     </row>
     <row r="4">
@@ -497,11 +497,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_AP.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AP.csv.gz</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>233785</v>
+        <v>234207</v>
       </c>
     </row>
     <row r="5">
@@ -515,11 +515,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_AM.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AM.csv.gz</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1008019</v>
+        <v>1019536</v>
       </c>
     </row>
     <row r="6">
@@ -533,11 +533,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_BA.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_BA.csv.gz</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>5050941</v>
+        <v>5084237</v>
       </c>
     </row>
     <row r="7">
@@ -551,11 +551,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_CE.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_CE.csv.gz</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2638321</v>
+        <v>2645740</v>
       </c>
     </row>
     <row r="8">
@@ -569,11 +569,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_DF.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_DF.csv.gz</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>100876</v>
+        <v>102000</v>
       </c>
     </row>
     <row r="9">
@@ -587,11 +587,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_ES.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_ES.csv.gz</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1241045</v>
+        <v>1248800</v>
       </c>
     </row>
     <row r="10">
@@ -605,11 +605,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_GO.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_GO.csv.gz</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1958069</v>
+        <v>1966481</v>
       </c>
     </row>
     <row r="11">
@@ -623,11 +623,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_MA.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MA.csv.gz</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2543477</v>
+        <v>2548231</v>
       </c>
     </row>
     <row r="12">
@@ -641,11 +641,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_MT.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MT.csv.gz</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1291228</v>
+        <v>1296558</v>
       </c>
     </row>
     <row r="13">
@@ -659,11 +659,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_MS.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MS.csv.gz</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>972875</v>
+        <v>976936</v>
       </c>
     </row>
     <row r="14">
@@ -677,11 +677,11 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_MG.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MG.csv.gz</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>7037785</v>
+        <v>7071457</v>
       </c>
     </row>
     <row r="15">
@@ -695,11 +695,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PA.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PA.csv.gz</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2303752</v>
+        <v>2308189</v>
       </c>
     </row>
     <row r="16">
@@ -713,11 +713,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PB.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PB.csv.gz</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1574045</v>
+        <v>1581090</v>
       </c>
     </row>
     <row r="17">
@@ -731,11 +731,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PR.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PR.csv.gz</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3339188</v>
+        <v>3344884</v>
       </c>
     </row>
     <row r="18">
@@ -749,11 +749,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PE.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PE.csv.gz</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3054336</v>
+        <v>3071745</v>
       </c>
     </row>
     <row r="19">
@@ -767,11 +767,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PI.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PI.csv.gz</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1301116</v>
+        <v>1308471</v>
       </c>
     </row>
     <row r="20">
@@ -785,11 +785,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RJ.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RJ.csv.gz</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2095500</v>
+        <v>2110560</v>
       </c>
     </row>
     <row r="21">
@@ -803,11 +803,11 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RN.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RN.csv.gz</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1516904</v>
+        <v>1522529</v>
       </c>
     </row>
     <row r="22">
@@ -821,11 +821,11 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RS.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RS.csv.gz</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3696286</v>
+        <v>3710549</v>
       </c>
     </row>
     <row r="23">
@@ -839,11 +839,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RO.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RO.csv.gz</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>534013</v>
+        <v>536935</v>
       </c>
     </row>
     <row r="24">
@@ -857,11 +857,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RR.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RR.csv.gz</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>195619</v>
+        <v>197379</v>
       </c>
     </row>
     <row r="25">
@@ -875,11 +875,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_SC.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SC.csv.gz</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2503854</v>
+        <v>2512839</v>
       </c>
     </row>
     <row r="26">
@@ -893,11 +893,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_SP.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SP.csv.gz</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>9111079</v>
+        <v>9202153</v>
       </c>
     </row>
     <row r="27">
@@ -911,11 +911,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_SE.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SE.csv.gz</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>859543</v>
+        <v>864669</v>
       </c>
     </row>
     <row r="28">
@@ -929,11 +929,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_TO.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_TO.csv.gz</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>743866</v>
+        <v>746663</v>
       </c>
     </row>
     <row r="29">
@@ -947,11 +947,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_AC.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AC.csv.gz</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>350298</v>
+        <v>352928</v>
       </c>
     </row>
     <row r="30">
@@ -965,11 +965,11 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_AL.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AL.csv.gz</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1067917</v>
+        <v>1072791</v>
       </c>
     </row>
     <row r="31">
@@ -983,11 +983,11 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_AP.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AP.csv.gz</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>233785</v>
+        <v>234207</v>
       </c>
     </row>
     <row r="32">
@@ -1001,11 +1001,11 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_AM.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AM.csv.gz</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1008019</v>
+        <v>1019536</v>
       </c>
     </row>
     <row r="33">
@@ -1019,11 +1019,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_BA.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_BA.csv.gz</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>5050941</v>
+        <v>5084237</v>
       </c>
     </row>
     <row r="34">
@@ -1037,11 +1037,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_CE.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_CE.csv.gz</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2638321</v>
+        <v>2645740</v>
       </c>
     </row>
     <row r="35">
@@ -1055,11 +1055,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_DF.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_DF.csv.gz</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>100876</v>
+        <v>102000</v>
       </c>
     </row>
     <row r="36">
@@ -1073,11 +1073,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_ES.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_ES.csv.gz</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1241045</v>
+        <v>1248800</v>
       </c>
     </row>
     <row r="37">
@@ -1091,11 +1091,11 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_GO.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_GO.csv.gz</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1958069</v>
+        <v>1966481</v>
       </c>
     </row>
     <row r="38">
@@ -1109,11 +1109,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_MA.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MA.csv.gz</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2543477</v>
+        <v>2548231</v>
       </c>
     </row>
     <row r="39">
@@ -1127,11 +1127,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_MT.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MT.csv.gz</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1291228</v>
+        <v>1296558</v>
       </c>
     </row>
     <row r="40">
@@ -1145,11 +1145,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_MS.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MS.csv.gz</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>972875</v>
+        <v>976936</v>
       </c>
     </row>
     <row r="41">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_MG.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MG.csv.gz</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>7037785</v>
+        <v>7071457</v>
       </c>
     </row>
     <row r="42">
@@ -1181,11 +1181,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PA.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PA.csv.gz</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>2303752</v>
+        <v>2308189</v>
       </c>
     </row>
     <row r="43">
@@ -1199,11 +1199,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PB.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PB.csv.gz</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1574045</v>
+        <v>1581090</v>
       </c>
     </row>
     <row r="44">
@@ -1217,11 +1217,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PR.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PR.csv.gz</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>3339188</v>
+        <v>3344884</v>
       </c>
     </row>
     <row r="45">
@@ -1235,11 +1235,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PE.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PE.csv.gz</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>3054336</v>
+        <v>3071745</v>
       </c>
     </row>
     <row r="46">
@@ -1253,11 +1253,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_PI.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PI.csv.gz</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1301116</v>
+        <v>1308471</v>
       </c>
     </row>
     <row r="47">
@@ -1271,11 +1271,11 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RJ.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RJ.csv.gz</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2095500</v>
+        <v>2110560</v>
       </c>
     </row>
     <row r="48">
@@ -1289,11 +1289,11 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RN.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RN.csv.gz</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1516904</v>
+        <v>1522529</v>
       </c>
     </row>
     <row r="49">
@@ -1307,11 +1307,11 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RS.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RS.csv.gz</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>3696286</v>
+        <v>3710549</v>
       </c>
     </row>
     <row r="50">
@@ -1325,11 +1325,11 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RO.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RO.csv.gz</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>534013</v>
+        <v>536935</v>
       </c>
     </row>
     <row r="51">
@@ -1343,11 +1343,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_RR.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RR.csv.gz</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>195619</v>
+        <v>197379</v>
       </c>
     </row>
     <row r="52">
@@ -1361,11 +1361,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_SC.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SC.csv.gz</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2503854</v>
+        <v>2512839</v>
       </c>
     </row>
     <row r="53">
@@ -1379,11 +1379,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_SP.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SP.csv.gz</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>9111079</v>
+        <v>9202153</v>
       </c>
     </row>
     <row r="54">
@@ -1397,11 +1397,11 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_SE.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SE.csv.gz</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>859543</v>
+        <v>864669</v>
       </c>
     </row>
     <row r="55">
@@ -1415,11 +1415,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/processed_TO.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_TO.csv.gz</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>743866</v>
+        <v>746663</v>
       </c>
     </row>
     <row r="56">
@@ -1433,11 +1433,11 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2020.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2020.csv.gz</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>1314339</v>
+        <v>1314380</v>
       </c>
     </row>
     <row r="57">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2021.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2021.csv.gz</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1469,11 +1469,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time.csv.gz</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>1679100</v>
+        <v>1701488</v>
       </c>
     </row>
     <row r="59">
@@ -1487,11 +1487,11 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2020.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2020.csv.gz</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>1314339</v>
+        <v>1314380</v>
       </c>
     </row>
     <row r="60">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2021.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2021.csv.gz</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1523,11 +1523,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>/home/pedro/Documentos/Doutorado/MO412/final_project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time.csv.gz</t>
+          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time.csv.gz</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>1679100</v>
+        <v>1701488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementing improvement of vaccination proximity
</commit_message>
<xml_diff>
--- a/data/output/processing_statistics.xlsx
+++ b/data/output/processing_statistics.xlsx
@@ -461,11 +461,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AC.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_AC.csv.gz</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>352928</v>
+        <v>354957</v>
       </c>
     </row>
     <row r="3">
@@ -479,11 +479,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AL.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_AL.csv.gz</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1072791</v>
+        <v>1077268</v>
       </c>
     </row>
     <row r="4">
@@ -497,11 +497,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AP.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_AP.csv.gz</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>234207</v>
+        <v>236189</v>
       </c>
     </row>
     <row r="5">
@@ -515,11 +515,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AM.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_AM.csv.gz</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1019536</v>
+        <v>1026741</v>
       </c>
     </row>
     <row r="6">
@@ -533,11 +533,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_BA.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_BA.csv.gz</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>5084237</v>
+        <v>5109864</v>
       </c>
     </row>
     <row r="7">
@@ -551,11 +551,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_CE.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_CE.csv.gz</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2645740</v>
+        <v>2660820</v>
       </c>
     </row>
     <row r="8">
@@ -569,11 +569,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_DF.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_DF.csv.gz</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>102000</v>
+        <v>103065</v>
       </c>
     </row>
     <row r="9">
@@ -587,11 +587,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_ES.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_ES.csv.gz</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1248800</v>
+        <v>1252587</v>
       </c>
     </row>
     <row r="10">
@@ -605,11 +605,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_GO.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_GO.csv.gz</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1966481</v>
+        <v>1973666</v>
       </c>
     </row>
     <row r="11">
@@ -623,11 +623,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MA.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_MA.csv.gz</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2548231</v>
+        <v>2557270</v>
       </c>
     </row>
     <row r="12">
@@ -641,11 +641,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MT.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_MT.csv.gz</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1296558</v>
+        <v>1301109</v>
       </c>
     </row>
     <row r="13">
@@ -659,11 +659,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MS.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_MS.csv.gz</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>976936</v>
+        <v>979687</v>
       </c>
     </row>
     <row r="14">
@@ -677,11 +677,11 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MG.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_MG.csv.gz</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>7071457</v>
+        <v>7097066</v>
       </c>
     </row>
     <row r="15">
@@ -695,11 +695,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PA.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PA.csv.gz</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2308189</v>
+        <v>2323741</v>
       </c>
     </row>
     <row r="16">
@@ -713,11 +713,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PB.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PB.csv.gz</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1581090</v>
+        <v>1585074</v>
       </c>
     </row>
     <row r="17">
@@ -731,11 +731,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PR.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PR.csv.gz</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3344884</v>
+        <v>3361230</v>
       </c>
     </row>
     <row r="18">
@@ -749,11 +749,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PE.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PE.csv.gz</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3071745</v>
+        <v>3085171</v>
       </c>
     </row>
     <row r="19">
@@ -767,11 +767,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PI.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PI.csv.gz</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1308471</v>
+        <v>1314846</v>
       </c>
     </row>
     <row r="20">
@@ -785,11 +785,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RJ.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RJ.csv.gz</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2110560</v>
+        <v>2124822</v>
       </c>
     </row>
     <row r="21">
@@ -803,11 +803,11 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RN.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RN.csv.gz</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1522529</v>
+        <v>1530749</v>
       </c>
     </row>
     <row r="22">
@@ -821,11 +821,11 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RS.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RS.csv.gz</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3710549</v>
+        <v>3724089</v>
       </c>
     </row>
     <row r="23">
@@ -839,11 +839,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RO.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RO.csv.gz</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>536935</v>
+        <v>539053</v>
       </c>
     </row>
     <row r="24">
@@ -857,11 +857,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RR.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RR.csv.gz</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>197379</v>
+        <v>199068</v>
       </c>
     </row>
     <row r="25">
@@ -875,11 +875,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SC.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_SC.csv.gz</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2512839</v>
+        <v>2520609</v>
       </c>
     </row>
     <row r="26">
@@ -893,11 +893,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SP.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_SP.csv.gz</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>9202153</v>
+        <v>9255253</v>
       </c>
     </row>
     <row r="27">
@@ -911,11 +911,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SE.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_SE.csv.gz</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>864669</v>
+        <v>868964</v>
       </c>
     </row>
     <row r="28">
@@ -929,11 +929,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_TO.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_TO.csv.gz</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>746663</v>
+        <v>748616</v>
       </c>
     </row>
     <row r="29">
@@ -947,11 +947,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AC.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_AC.csv.gz</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>352928</v>
+        <v>354957</v>
       </c>
     </row>
     <row r="30">
@@ -965,11 +965,11 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AL.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_AL.csv.gz</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1072791</v>
+        <v>1077268</v>
       </c>
     </row>
     <row r="31">
@@ -983,11 +983,11 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AP.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_AP.csv.gz</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>234207</v>
+        <v>236189</v>
       </c>
     </row>
     <row r="32">
@@ -1001,11 +1001,11 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_AM.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_AM.csv.gz</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1019536</v>
+        <v>1026741</v>
       </c>
     </row>
     <row r="33">
@@ -1019,11 +1019,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_BA.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_BA.csv.gz</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>5084237</v>
+        <v>5109864</v>
       </c>
     </row>
     <row r="34">
@@ -1037,11 +1037,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_CE.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_CE.csv.gz</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2645740</v>
+        <v>2660820</v>
       </c>
     </row>
     <row r="35">
@@ -1055,11 +1055,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_DF.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_DF.csv.gz</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>102000</v>
+        <v>103065</v>
       </c>
     </row>
     <row r="36">
@@ -1073,11 +1073,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_ES.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_ES.csv.gz</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1248800</v>
+        <v>1252587</v>
       </c>
     </row>
     <row r="37">
@@ -1091,11 +1091,11 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_GO.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_GO.csv.gz</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1966481</v>
+        <v>1973666</v>
       </c>
     </row>
     <row r="38">
@@ -1109,11 +1109,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MA.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_MA.csv.gz</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2548231</v>
+        <v>2557270</v>
       </c>
     </row>
     <row r="39">
@@ -1127,11 +1127,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MT.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_MT.csv.gz</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1296558</v>
+        <v>1301109</v>
       </c>
     </row>
     <row r="40">
@@ -1145,11 +1145,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MS.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_MS.csv.gz</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>976936</v>
+        <v>979687</v>
       </c>
     </row>
     <row r="41">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_MG.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_MG.csv.gz</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>7071457</v>
+        <v>7097066</v>
       </c>
     </row>
     <row r="42">
@@ -1181,11 +1181,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PA.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PA.csv.gz</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>2308189</v>
+        <v>2323741</v>
       </c>
     </row>
     <row r="43">
@@ -1199,11 +1199,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PB.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PB.csv.gz</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1581090</v>
+        <v>1585074</v>
       </c>
     </row>
     <row r="44">
@@ -1217,11 +1217,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PR.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PR.csv.gz</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>3344884</v>
+        <v>3361230</v>
       </c>
     </row>
     <row r="45">
@@ -1235,11 +1235,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PE.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PE.csv.gz</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>3071745</v>
+        <v>3085171</v>
       </c>
     </row>
     <row r="46">
@@ -1253,11 +1253,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_PI.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_PI.csv.gz</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1308471</v>
+        <v>1314846</v>
       </c>
     </row>
     <row r="47">
@@ -1271,11 +1271,11 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RJ.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RJ.csv.gz</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2110560</v>
+        <v>2124822</v>
       </c>
     </row>
     <row r="48">
@@ -1289,11 +1289,11 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RN.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RN.csv.gz</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1522529</v>
+        <v>1530749</v>
       </c>
     </row>
     <row r="49">
@@ -1307,11 +1307,11 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RS.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RS.csv.gz</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>3710549</v>
+        <v>3724089</v>
       </c>
     </row>
     <row r="50">
@@ -1325,11 +1325,11 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RO.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RO.csv.gz</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>536935</v>
+        <v>539053</v>
       </c>
     </row>
     <row r="51">
@@ -1343,11 +1343,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_RR.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_RR.csv.gz</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>197379</v>
+        <v>199068</v>
       </c>
     </row>
     <row r="52">
@@ -1361,11 +1361,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SC.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_SC.csv.gz</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2512839</v>
+        <v>2520609</v>
       </c>
     </row>
     <row r="53">
@@ -1379,11 +1379,11 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SP.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_SP.csv.gz</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>9202153</v>
+        <v>9255253</v>
       </c>
     </row>
     <row r="54">
@@ -1397,11 +1397,11 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_SE.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_SE.csv.gz</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>864669</v>
+        <v>868964</v>
       </c>
     </row>
     <row r="55">
@@ -1415,11 +1415,11 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/processed_TO.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/processed_TO.csv.gz</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>746663</v>
+        <v>748616</v>
       </c>
     </row>
     <row r="56">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2020.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2020.csv.gz</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2021.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2021.csv.gz</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1469,11 +1469,11 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time.csv.gz</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>1701488</v>
+        <v>1751861</v>
       </c>
     </row>
     <row r="59">
@@ -1487,7 +1487,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2020.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2020.csv.gz</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2021.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time_2021.csv.gz</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1523,11 +1523,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>C:/Users/Pedro/Documents/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time.csv.gz</t>
+          <t>W:/Meu Drive/Doutorado IC-Unicamp/MO412 - Graphs Algorithms/07. Final Project/Covid19VaccinationProject/source/../data/input/cases-brazil-cities-time.csv.gz</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>1701488</v>
+        <v>1751861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>